<commit_message>
waiting time su response time impatto
</commit_message>
<xml_diff>
--- a/analysis/analisiFattoriale-tmkX/factorialAnalysis.xlsx
+++ b/analysis/analisiFattoriale-tmkX/factorialAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Poggiani\Documents\GitHub\PECSNproject\analysis\analisiFattoriale-tmkX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3244C8C7-FA27-4ACF-ABE8-2DC9D3302C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2582F974-12A7-4A79-B77F-1E6844EED983}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1032" yWindow="2508" windowWidth="18600" windowHeight="10044" xr2:uid="{D66025A6-D572-40D5-92B3-954676799273}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{D66025A6-D572-40D5-92B3-954676799273}"/>
   </bookViews>
   <sheets>
     <sheet name="Factorial Analysis" sheetId="1" r:id="rId1"/>
@@ -535,6 +535,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -545,12 +551,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3113,7 +3113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE93E289-3EE5-4135-BF41-859E3A8B782C}">
   <dimension ref="A1:AH143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -6976,18 +6976,18 @@
       <c r="B11">
         <v>400</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30" t="s">
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -6996,22 +6996,22 @@
       <c r="B12">
         <v>10</v>
       </c>
-      <c r="J12" s="31" t="s">
+      <c r="J12" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31" t="s">
+      <c r="K12" s="27"/>
+      <c r="L12" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31" t="s">
+      <c r="M12" s="27"/>
+      <c r="N12" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31" t="s">
+      <c r="O12" s="27"/>
+      <c r="P12" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="Q12" s="31"/>
+      <c r="Q12" s="27"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -7020,11 +7020,11 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
       <c r="J13" s="16" t="s">
         <v>55</v>
       </c>
@@ -7057,11 +7057,11 @@
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
       <c r="J14" s="15">
         <v>7.5307516287585405E-2</v>
       </c>
@@ -7088,11 +7088,11 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -7122,9 +7122,9 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -7138,9 +7138,9 @@
       <c r="Q16" s="17"/>
     </row>
     <row r="17" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -7155,18 +7155,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="J11:M11"/>
     <mergeCell ref="N11:Q11"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="L12:M12"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
analisi fattoriale 2 fattori
</commit_message>
<xml_diff>
--- a/analysis/analisiFattoriale-tmkX/factorialAnalysis.xlsx
+++ b/analysis/analisiFattoriale-tmkX/factorialAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Poggiani\Documents\GitHub\PECSNproject\analysis\analisiFattoriale-tmkX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2582F974-12A7-4A79-B77F-1E6844EED983}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519AB1C7-9F97-4380-A98F-D646562A6C74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{D66025A6-D572-40D5-92B3-954676799273}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="62">
   <si>
     <t>k</t>
   </si>
@@ -72,9 +72,6 @@
     <t>{0.5, 4}</t>
   </si>
   <si>
-    <t>Memory size (MB) A</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -87,58 +84,7 @@
     <t>AB</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Cache size (MB) B</t>
-  </si>
-  <si>
-    <t>(yi - y_)^2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y_ = </t>
-  </si>
-  <si>
-    <t>TOTALE:</t>
-  </si>
-  <si>
     <t>4*qi^2</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>es2</t>
-  </si>
-  <si>
-    <t>Errors</t>
-  </si>
-  <si>
-    <t>y1</t>
-  </si>
-  <si>
-    <t>y2</t>
-  </si>
-  <si>
-    <t>y3</t>
-  </si>
-  <si>
-    <t>Y_</t>
-  </si>
-  <si>
-    <t>y1-y_</t>
-  </si>
-  <si>
-    <t>y2-y_</t>
-  </si>
-  <si>
-    <t>y3-y_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">totale: </t>
-  </si>
-  <si>
-    <t>4*3*qi^2</t>
   </si>
   <si>
     <t>Q</t>
@@ -314,7 +260,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +312,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -535,12 +487,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -553,6 +499,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3113,8 +3066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE93E289-3EE5-4135-BF41-859E3A8B782C}">
   <dimension ref="A1:AH143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="L73" sqref="L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3130,83 +3083,83 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B1" s="24"/>
       <c r="G1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="M1" s="8" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="U1" s="19" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="V1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="AB1" s="8" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="AC1" s="8" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="AE1" s="8" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="AF1" s="8" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="AH1" s="8" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
@@ -3466,7 +3419,7 @@
         <v>5.1308187288137401E-2</v>
       </c>
       <c r="W4" s="13">
-        <f t="shared" ref="W4:W17" si="15">H4*$AH4</f>
+        <f>H4*$AH4</f>
         <v>-5.1308187288137401E-2</v>
       </c>
       <c r="X4" s="13">
@@ -3482,7 +3435,7 @@
         <v>-5.1308187288137401E-2</v>
       </c>
       <c r="AA4" s="13">
-        <f t="shared" ref="AA4:AA17" si="16">W4*X4</f>
+        <f t="shared" ref="AA4:AA17" si="15">W4*X4</f>
         <v>-2.6325300827945842E-3</v>
       </c>
       <c r="AB4" s="13">
@@ -3566,7 +3519,7 @@
         <v>0.45210537717229898</v>
       </c>
       <c r="W5" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="W4:W17" si="16">H5*$AH5</f>
         <v>-0.45210537717229898</v>
       </c>
       <c r="X5" s="13">
@@ -3582,7 +3535,7 @@
         <v>-0.45210537717229898</v>
       </c>
       <c r="AA5" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>-0.20439927206810674</v>
       </c>
       <c r="AB5" s="13">
@@ -3611,7 +3564,7 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
@@ -3666,7 +3619,7 @@
         <v>7.7558958472437503E-2</v>
       </c>
       <c r="W6" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.7558958472437503E-2</v>
       </c>
       <c r="X6" s="13">
@@ -3682,7 +3635,7 @@
         <v>-7.7558958472437503E-2</v>
       </c>
       <c r="AA6" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>-6.0153920393292851E-3</v>
       </c>
       <c r="AB6" s="13">
@@ -3757,7 +3710,7 @@
         <v>0.13962808226922699</v>
       </c>
       <c r="W7" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.13962808226922699</v>
       </c>
       <c r="X7" s="13">
@@ -3773,7 +3726,7 @@
         <v>-0.13962808226922699</v>
       </c>
       <c r="AA7" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>-1.9496001358182021E-2</v>
       </c>
       <c r="AB7" s="13">
@@ -3802,7 +3755,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3851,7 +3804,7 @@
         <v>4.7559191730608102E-2</v>
       </c>
       <c r="W8" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.7559191730608102E-2</v>
       </c>
       <c r="X8" s="13">
@@ -3867,7 +3820,7 @@
         <v>-4.7559191730608102E-2</v>
       </c>
       <c r="AA8" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2.261876718068742E-3</v>
       </c>
       <c r="AB8" s="13">
@@ -3896,7 +3849,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -3948,7 +3901,7 @@
         <v>0.484366960427631</v>
       </c>
       <c r="W9" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.484366960427631</v>
       </c>
       <c r="X9" s="13">
@@ -3964,7 +3917,7 @@
         <v>-0.484366960427631</v>
       </c>
       <c r="AA9" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.23461135235390226</v>
       </c>
       <c r="AB9" s="13">
@@ -3993,10 +3946,10 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -4045,7 +3998,7 @@
         <v>3.6770684894178299E-2</v>
       </c>
       <c r="W10" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.6770684894178299E-2</v>
       </c>
       <c r="X10" s="13">
@@ -4061,7 +4014,7 @@
         <v>3.6770684894178299E-2</v>
       </c>
       <c r="AA10" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>1.3520832675869522E-3</v>
       </c>
       <c r="AB10" s="13">
@@ -4090,7 +4043,7 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -4142,7 +4095,7 @@
         <v>0.13708566577607501</v>
       </c>
       <c r="W11" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-0.13708566577607501</v>
       </c>
       <c r="X11" s="13">
@@ -4158,7 +4111,7 @@
         <v>0.13708566577607501</v>
       </c>
       <c r="AA11" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>1.8792479761269743E-2</v>
       </c>
       <c r="AB11" s="13">
@@ -4187,7 +4140,7 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -4239,7 +4192,7 @@
         <v>3.9512073636022903E-2</v>
       </c>
       <c r="W12" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.9512073636022903E-2</v>
       </c>
       <c r="X12" s="13">
@@ -4255,7 +4208,7 @@
         <v>3.9512073636022903E-2</v>
       </c>
       <c r="AA12" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>-1.5612039630184961E-3</v>
       </c>
       <c r="AB12" s="13">
@@ -4330,7 +4283,7 @@
         <v>0.21247080756198999</v>
       </c>
       <c r="W13" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-0.21247080756198999</v>
       </c>
       <c r="X13" s="13">
@@ -4346,7 +4299,7 @@
         <v>0.21247080756198999</v>
       </c>
       <c r="AA13" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>-4.5143844066044186E-2</v>
       </c>
       <c r="AB13" s="13">
@@ -4421,7 +4374,7 @@
         <v>3.6208083767558102E-2</v>
       </c>
       <c r="W14" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.6208083767558102E-2</v>
       </c>
       <c r="X14" s="13">
@@ -4437,7 +4390,7 @@
         <v>3.6208083767558102E-2</v>
       </c>
       <c r="AA14" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>-1.3110253301185045E-3</v>
       </c>
       <c r="AB14" s="13">
@@ -4512,7 +4465,7 @@
         <v>0.13742001360839101</v>
       </c>
       <c r="W15" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.13742001360839101</v>
       </c>
       <c r="X15" s="13">
@@ -4528,7 +4481,7 @@
         <v>0.13742001360839101</v>
       </c>
       <c r="AA15" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>-1.8884260140130373E-2</v>
       </c>
       <c r="AB15" s="13">
@@ -4603,7 +4556,7 @@
         <v>3.88719092150146E-2</v>
       </c>
       <c r="W16" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.88719092150146E-2</v>
       </c>
       <c r="X16" s="13">
@@ -4619,7 +4572,7 @@
         <v>3.88719092150146E-2</v>
       </c>
       <c r="AA16" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>1.5110253260203369E-3</v>
       </c>
       <c r="AB16" s="13">
@@ -4694,7 +4647,7 @@
         <v>0.211278284021195</v>
       </c>
       <c r="W17" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.211278284021195</v>
       </c>
       <c r="X17" s="13">
@@ -4710,7 +4663,7 @@
         <v>0.211278284021195</v>
       </c>
       <c r="AA17" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4.4638513298940745E-2</v>
       </c>
       <c r="AB17" s="13">
@@ -4739,7 +4692,7 @@
     </row>
     <row r="18" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="R18" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="S18">
         <f>SUM(S2:S17)</f>
@@ -4748,7 +4701,7 @@
     </row>
     <row r="19" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F19" s="21" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="G19" s="20">
         <f>SUM(S2:S17)</f>
@@ -4795,7 +4748,7 @@
         <v>-0.42625278863972965</v>
       </c>
       <c r="R19" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="S19">
         <f>S18/16</f>
@@ -4804,7 +4757,7 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G20">
         <f>G19/16</f>
@@ -4851,12 +4804,12 @@
         <v>-2.6640799289983103E-2</v>
       </c>
       <c r="R20" s="19" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="H21">
         <f>4*100*(H20)^2</f>
@@ -4904,7 +4857,7 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="H22">
         <f>(H21/$S$23)*100</f>
@@ -4953,7 +4906,7 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="R23" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="S23">
         <f>SUM(H21:Q21,R21)</f>
@@ -4962,43 +4915,46 @@
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B27" s="24"/>
       <c r="G27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="I27" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="J27" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="M27" s="8" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="P27" s="8" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="Q27" s="8" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="R27" s="8"/>
+      <c r="S27" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G28">
@@ -5040,6 +4996,9 @@
         <f>J28*K28</f>
         <v>1</v>
       </c>
+      <c r="S28">
+        <v>7.5307516287585405E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G29">
@@ -5081,6 +5040,9 @@
         <f t="shared" ref="Q29:Q43" si="32">J29*K29</f>
         <v>-1</v>
       </c>
+      <c r="S29" s="15">
+        <v>0.13559242462957</v>
+      </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G30">
@@ -5122,6 +5084,9 @@
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
+      <c r="S30" s="15">
+        <v>5.1308187288137401E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G31">
@@ -5163,6 +5128,9 @@
         <f t="shared" si="32"/>
         <v>-1</v>
       </c>
+      <c r="S31" s="15">
+        <v>0.45210537717229898</v>
+      </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G32">
@@ -5204,6 +5172,9 @@
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
+      <c r="S32" s="15">
+        <v>7.7558958472437503E-2</v>
+      </c>
     </row>
     <row r="33" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G33">
@@ -5245,6 +5216,9 @@
         <f t="shared" si="32"/>
         <v>-1</v>
       </c>
+      <c r="S33" s="15">
+        <v>0.13962808226922699</v>
+      </c>
     </row>
     <row r="34" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G34">
@@ -5286,6 +5260,9 @@
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
+      <c r="S34" s="15">
+        <v>4.7559191730608102E-2</v>
+      </c>
     </row>
     <row r="35" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G35">
@@ -5327,6 +5304,9 @@
         <f t="shared" si="32"/>
         <v>-1</v>
       </c>
+      <c r="S35" s="15">
+        <v>0.484366960427631</v>
+      </c>
     </row>
     <row r="36" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G36">
@@ -5368,6 +5348,9 @@
         <f t="shared" si="32"/>
         <v>-1</v>
       </c>
+      <c r="S36" s="15">
+        <v>3.6770684894178299E-2</v>
+      </c>
     </row>
     <row r="37" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G37">
@@ -5409,6 +5392,9 @@
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
+      <c r="S37">
+        <v>0.13708566577607501</v>
+      </c>
     </row>
     <row r="38" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G38">
@@ -5450,6 +5436,9 @@
         <f t="shared" si="32"/>
         <v>-1</v>
       </c>
+      <c r="S38">
+        <v>3.9512073636022903E-2</v>
+      </c>
     </row>
     <row r="39" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G39">
@@ -5491,6 +5480,9 @@
         <f t="shared" si="32"/>
         <v>-1</v>
       </c>
+      <c r="S39">
+        <v>0.21247080756198999</v>
+      </c>
     </row>
     <row r="40" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G40">
@@ -5532,6 +5524,9 @@
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
+      <c r="S40" s="15">
+        <v>3.6208083767558102E-2</v>
+      </c>
     </row>
     <row r="41" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G41">
@@ -5573,6 +5568,9 @@
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
+      <c r="S41">
+        <v>0.13742001360839101</v>
+      </c>
     </row>
     <row r="42" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G42">
@@ -5614,6 +5612,9 @@
         <f t="shared" si="32"/>
         <v>-1</v>
       </c>
+      <c r="S42">
+        <v>3.88719092150146E-2</v>
+      </c>
     </row>
     <row r="43" spans="6:19" x14ac:dyDescent="0.3">
       <c r="G43">
@@ -5655,15 +5656,22 @@
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="6:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="S43">
+        <v>0.211278284021195</v>
+      </c>
+    </row>
+    <row r="44" spans="6:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S44">
+        <v>2.31304422075792</v>
+      </c>
+    </row>
     <row r="45" spans="6:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F45" s="21" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="G45" s="20">
         <f>SUM(S28:S43)</f>
-        <v>0</v>
+        <v>2.31304422075792</v>
       </c>
       <c r="H45" s="20">
         <v>3.2738746266204405E-2</v>
@@ -5696,14 +5704,17 @@
         <v>-0.42625278863972965</v>
       </c>
       <c r="R45" s="22"/>
+      <c r="S45">
+        <v>0.14456526379737</v>
+      </c>
     </row>
     <row r="46" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F46" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="G46">
         <f>G45/16</f>
-        <v>0</v>
+        <v>0.14456526379737</v>
       </c>
       <c r="H46">
         <v>2.0461716416377753E-3</v>
@@ -5742,7 +5753,7 @@
     </row>
     <row r="47" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F47" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H47">
         <f>4*(H46)^2</f>
@@ -5787,7 +5798,7 @@
     </row>
     <row r="48" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F48" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="H48">
         <f>(H47/$S$46)*100</f>
@@ -5830,7 +5841,7 @@
         <v>6.6287833687672384</v>
       </c>
     </row>
-    <row r="49" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.3">
       <c r="F49" s="23"/>
       <c r="G49" s="23"/>
       <c r="H49" s="23"/>
@@ -5845,717 +5856,1423 @@
       <c r="Q49" s="23"/>
       <c r="R49" s="23"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B65" s="25" t="s">
+    <row r="50" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="H51" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M51" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="8"/>
+      <c r="R51" s="8"/>
+      <c r="V51" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="W51" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="X51" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y51" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z51" s="8"/>
+      <c r="AA51" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB51" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC51" s="8"/>
+      <c r="AD51" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE51" s="8"/>
+      <c r="AF51" s="8"/>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I52" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J52" s="13">
+        <v>-1</v>
+      </c>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13">
+        <f>H52*I52</f>
+        <v>1</v>
+      </c>
+      <c r="M52" s="13">
+        <f>H52*J52</f>
+        <v>1</v>
+      </c>
+      <c r="N52" s="13"/>
+      <c r="O52" s="13">
+        <f>I52*J52</f>
+        <v>1</v>
+      </c>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="13"/>
+      <c r="S52">
+        <v>7.5307516287585405E-2</v>
+      </c>
+      <c r="V52">
+        <f>G52*$S52</f>
+        <v>7.5307516287585405E-2</v>
+      </c>
+      <c r="W52">
+        <f t="shared" ref="W52:AD67" si="37">H52*$S52</f>
+        <v>-7.5307516287585405E-2</v>
+      </c>
+      <c r="X52">
+        <f t="shared" si="37"/>
+        <v>-7.5307516287585405E-2</v>
+      </c>
+      <c r="Y52">
+        <f t="shared" si="37"/>
+        <v>-7.5307516287585405E-2</v>
+      </c>
+      <c r="Z52">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA52">
+        <f t="shared" si="37"/>
+        <v>7.5307516287585405E-2</v>
+      </c>
+      <c r="AB52">
+        <f t="shared" si="37"/>
+        <v>7.5307516287585405E-2</v>
+      </c>
+      <c r="AC52">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD52">
+        <f t="shared" si="37"/>
+        <v>7.5307516287585405E-2</v>
+      </c>
+      <c r="AE52" s="13"/>
+      <c r="AF52" s="13"/>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I53" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J53" s="13">
+        <v>1</v>
+      </c>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13">
+        <f>H53*I53</f>
+        <v>1</v>
+      </c>
+      <c r="M53" s="13">
+        <f t="shared" ref="M53:M63" si="38">H53*J53</f>
+        <v>-1</v>
+      </c>
+      <c r="N53" s="13"/>
+      <c r="O53" s="13">
+        <f t="shared" ref="O53:O67" si="39">I53*J53</f>
+        <v>-1</v>
+      </c>
+      <c r="P53" s="13"/>
+      <c r="Q53" s="13"/>
+      <c r="S53" s="15">
+        <v>0.13559242462957</v>
+      </c>
+      <c r="V53">
+        <f t="shared" ref="V53:V67" si="40">G53*$S53</f>
+        <v>0.13559242462957</v>
+      </c>
+      <c r="W53">
+        <f t="shared" si="37"/>
+        <v>-0.13559242462957</v>
+      </c>
+      <c r="X53">
+        <f t="shared" si="37"/>
+        <v>-0.13559242462957</v>
+      </c>
+      <c r="Y53">
+        <f t="shared" si="37"/>
+        <v>0.13559242462957</v>
+      </c>
+      <c r="Z53">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA53">
+        <f t="shared" si="37"/>
+        <v>0.13559242462957</v>
+      </c>
+      <c r="AB53">
+        <f t="shared" si="37"/>
+        <v>-0.13559242462957</v>
+      </c>
+      <c r="AC53">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD53">
+        <f t="shared" si="37"/>
+        <v>-0.13559242462957</v>
+      </c>
+      <c r="AE53" s="13"/>
+      <c r="AF53" s="13"/>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I54" s="13">
+        <v>1</v>
+      </c>
+      <c r="J54" s="13">
+        <v>-1</v>
+      </c>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13">
+        <f t="shared" ref="L54:L67" si="41">H54*I54</f>
+        <v>-1</v>
+      </c>
+      <c r="M54" s="13">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="N54" s="13"/>
+      <c r="O54" s="13">
+        <f t="shared" si="39"/>
+        <v>-1</v>
+      </c>
+      <c r="P54" s="13"/>
+      <c r="Q54" s="13"/>
+      <c r="S54" s="15">
+        <v>5.1308187288137401E-2</v>
+      </c>
+      <c r="V54">
+        <f t="shared" si="40"/>
+        <v>5.1308187288137401E-2</v>
+      </c>
+      <c r="W54">
+        <f t="shared" si="37"/>
+        <v>-5.1308187288137401E-2</v>
+      </c>
+      <c r="X54">
+        <f t="shared" si="37"/>
+        <v>5.1308187288137401E-2</v>
+      </c>
+      <c r="Y54">
+        <f t="shared" si="37"/>
+        <v>-5.1308187288137401E-2</v>
+      </c>
+      <c r="Z54">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA54">
+        <f t="shared" si="37"/>
+        <v>-5.1308187288137401E-2</v>
+      </c>
+      <c r="AB54">
+        <f t="shared" si="37"/>
+        <v>5.1308187288137401E-2</v>
+      </c>
+      <c r="AC54">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD54">
+        <f t="shared" si="37"/>
+        <v>-5.1308187288137401E-2</v>
+      </c>
+      <c r="AE54" s="13"/>
+      <c r="AF54" s="13"/>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I55" s="13">
+        <v>1</v>
+      </c>
+      <c r="J55" s="13">
+        <v>1</v>
+      </c>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13">
+        <f t="shared" si="41"/>
+        <v>-1</v>
+      </c>
+      <c r="M55" s="13">
+        <f t="shared" si="38"/>
+        <v>-1</v>
+      </c>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="S55" s="15">
+        <v>0.45210537717229898</v>
+      </c>
+      <c r="V55">
+        <f t="shared" si="40"/>
+        <v>0.45210537717229898</v>
+      </c>
+      <c r="W55">
+        <f t="shared" si="37"/>
+        <v>-0.45210537717229898</v>
+      </c>
+      <c r="X55">
+        <f t="shared" si="37"/>
+        <v>0.45210537717229898</v>
+      </c>
+      <c r="Y55">
+        <f t="shared" si="37"/>
+        <v>0.45210537717229898</v>
+      </c>
+      <c r="Z55">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA55">
+        <f t="shared" si="37"/>
+        <v>-0.45210537717229898</v>
+      </c>
+      <c r="AB55">
+        <f t="shared" si="37"/>
+        <v>-0.45210537717229898</v>
+      </c>
+      <c r="AC55">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD55">
+        <f t="shared" si="37"/>
+        <v>0.45210537717229898</v>
+      </c>
+      <c r="AE55" s="13"/>
+      <c r="AF55" s="13"/>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" s="13">
+        <v>1</v>
+      </c>
+      <c r="I56" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J56" s="13">
+        <v>-1</v>
+      </c>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13">
+        <f t="shared" si="41"/>
+        <v>-1</v>
+      </c>
+      <c r="M56" s="13">
+        <f t="shared" si="38"/>
+        <v>-1</v>
+      </c>
+      <c r="N56" s="13"/>
+      <c r="O56" s="13">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="P56" s="13"/>
+      <c r="Q56" s="13"/>
+      <c r="S56" s="15">
+        <v>7.7558958472437503E-2</v>
+      </c>
+      <c r="V56">
+        <f t="shared" si="40"/>
+        <v>7.7558958472437503E-2</v>
+      </c>
+      <c r="W56">
+        <f t="shared" si="37"/>
+        <v>7.7558958472437503E-2</v>
+      </c>
+      <c r="X56">
+        <f t="shared" si="37"/>
+        <v>-7.7558958472437503E-2</v>
+      </c>
+      <c r="Y56">
+        <f t="shared" si="37"/>
+        <v>-7.7558958472437503E-2</v>
+      </c>
+      <c r="Z56">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA56">
+        <f t="shared" si="37"/>
+        <v>-7.7558958472437503E-2</v>
+      </c>
+      <c r="AB56">
+        <f t="shared" si="37"/>
+        <v>-7.7558958472437503E-2</v>
+      </c>
+      <c r="AC56">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD56">
+        <f t="shared" si="37"/>
+        <v>7.7558958472437503E-2</v>
+      </c>
+      <c r="AE56" s="13"/>
+      <c r="AF56" s="13"/>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" s="13">
+        <v>1</v>
+      </c>
+      <c r="I57" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J57" s="13">
+        <v>1</v>
+      </c>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13">
+        <f t="shared" si="41"/>
+        <v>-1</v>
+      </c>
+      <c r="M57" s="13">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13">
+        <f t="shared" si="39"/>
+        <v>-1</v>
+      </c>
+      <c r="P57" s="13"/>
+      <c r="Q57" s="13"/>
+      <c r="S57" s="15">
+        <v>0.13962808226922699</v>
+      </c>
+      <c r="V57">
+        <f t="shared" si="40"/>
+        <v>0.13962808226922699</v>
+      </c>
+      <c r="W57">
+        <f t="shared" si="37"/>
+        <v>0.13962808226922699</v>
+      </c>
+      <c r="X57">
+        <f t="shared" si="37"/>
+        <v>-0.13962808226922699</v>
+      </c>
+      <c r="Y57">
+        <f t="shared" si="37"/>
+        <v>0.13962808226922699</v>
+      </c>
+      <c r="Z57">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA57">
+        <f t="shared" si="37"/>
+        <v>-0.13962808226922699</v>
+      </c>
+      <c r="AB57">
+        <f t="shared" si="37"/>
+        <v>0.13962808226922699</v>
+      </c>
+      <c r="AC57">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD57">
+        <f t="shared" si="37"/>
+        <v>-0.13962808226922699</v>
+      </c>
+      <c r="AE57" s="13"/>
+      <c r="AF57" s="13"/>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" s="13">
+        <v>1</v>
+      </c>
+      <c r="I58" s="13">
+        <v>1</v>
+      </c>
+      <c r="J58" s="13">
+        <v>-1</v>
+      </c>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="M58" s="13">
+        <f t="shared" si="38"/>
+        <v>-1</v>
+      </c>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13">
+        <f t="shared" si="39"/>
+        <v>-1</v>
+      </c>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="S58" s="15">
+        <v>4.7559191730608102E-2</v>
+      </c>
+      <c r="V58">
+        <f t="shared" si="40"/>
+        <v>4.7559191730608102E-2</v>
+      </c>
+      <c r="W58">
+        <f t="shared" si="37"/>
+        <v>4.7559191730608102E-2</v>
+      </c>
+      <c r="X58">
+        <f t="shared" si="37"/>
+        <v>4.7559191730608102E-2</v>
+      </c>
+      <c r="Y58">
+        <f t="shared" si="37"/>
+        <v>-4.7559191730608102E-2</v>
+      </c>
+      <c r="Z58">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA58">
+        <f t="shared" si="37"/>
+        <v>4.7559191730608102E-2</v>
+      </c>
+      <c r="AB58">
+        <f t="shared" si="37"/>
+        <v>-4.7559191730608102E-2</v>
+      </c>
+      <c r="AC58">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD58">
+        <f t="shared" si="37"/>
+        <v>-4.7559191730608102E-2</v>
+      </c>
+      <c r="AE58" s="13"/>
+      <c r="AF58" s="13"/>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" s="13">
+        <v>1</v>
+      </c>
+      <c r="I59" s="13">
+        <v>1</v>
+      </c>
+      <c r="J59" s="13">
+        <v>1</v>
+      </c>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="M59" s="13">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="P59" s="13"/>
+      <c r="Q59" s="13"/>
+      <c r="S59" s="15">
+        <v>0.484366960427631</v>
+      </c>
+      <c r="V59">
+        <f t="shared" si="40"/>
+        <v>0.484366960427631</v>
+      </c>
+      <c r="W59">
+        <f t="shared" si="37"/>
+        <v>0.484366960427631</v>
+      </c>
+      <c r="X59">
+        <f t="shared" si="37"/>
+        <v>0.484366960427631</v>
+      </c>
+      <c r="Y59">
+        <f t="shared" si="37"/>
+        <v>0.484366960427631</v>
+      </c>
+      <c r="Z59">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA59">
+        <f t="shared" si="37"/>
+        <v>0.484366960427631</v>
+      </c>
+      <c r="AB59">
+        <f t="shared" si="37"/>
+        <v>0.484366960427631</v>
+      </c>
+      <c r="AC59">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD59">
+        <f t="shared" si="37"/>
+        <v>0.484366960427631</v>
+      </c>
+      <c r="AE59" s="13"/>
+      <c r="AF59" s="13"/>
+    </row>
+    <row r="60" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I60" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J60" s="13">
+        <v>-1</v>
+      </c>
+      <c r="K60" s="13"/>
+      <c r="L60" s="13">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="M60" s="13">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="N60" s="13"/>
+      <c r="O60" s="13">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="P60" s="13"/>
+      <c r="Q60" s="13"/>
+      <c r="S60" s="15">
+        <v>3.6770684894178299E-2</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="40"/>
+        <v>3.6770684894178299E-2</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="37"/>
+        <v>-3.6770684894178299E-2</v>
+      </c>
+      <c r="X60">
+        <f t="shared" si="37"/>
+        <v>-3.6770684894178299E-2</v>
+      </c>
+      <c r="Y60">
+        <f t="shared" si="37"/>
+        <v>-3.6770684894178299E-2</v>
+      </c>
+      <c r="Z60">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="37"/>
+        <v>3.6770684894178299E-2</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="37"/>
+        <v>3.6770684894178299E-2</v>
+      </c>
+      <c r="AC60">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD60">
+        <f t="shared" si="37"/>
+        <v>3.6770684894178299E-2</v>
+      </c>
+      <c r="AE60" s="13"/>
+      <c r="AF60" s="13"/>
+    </row>
+    <row r="61" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I61" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J61" s="13">
+        <v>1</v>
+      </c>
+      <c r="K61" s="13"/>
+      <c r="L61" s="13">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="M61" s="13">
+        <f t="shared" si="38"/>
+        <v>-1</v>
+      </c>
+      <c r="N61" s="13"/>
+      <c r="O61" s="13">
+        <f t="shared" si="39"/>
+        <v>-1</v>
+      </c>
+      <c r="P61" s="13"/>
+      <c r="Q61" s="13"/>
+      <c r="S61">
+        <v>0.13708566577607501</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="40"/>
+        <v>0.13708566577607501</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="37"/>
+        <v>-0.13708566577607501</v>
+      </c>
+      <c r="X61">
+        <f t="shared" si="37"/>
+        <v>-0.13708566577607501</v>
+      </c>
+      <c r="Y61">
+        <f t="shared" si="37"/>
+        <v>0.13708566577607501</v>
+      </c>
+      <c r="Z61">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA61">
+        <f t="shared" si="37"/>
+        <v>0.13708566577607501</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="37"/>
+        <v>-0.13708566577607501</v>
+      </c>
+      <c r="AC61">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD61">
+        <f t="shared" si="37"/>
+        <v>-0.13708566577607501</v>
+      </c>
+      <c r="AE61" s="13"/>
+      <c r="AF61" s="13"/>
+    </row>
+    <row r="62" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I62" s="13">
+        <v>1</v>
+      </c>
+      <c r="J62" s="13">
+        <v>-1</v>
+      </c>
+      <c r="K62" s="13"/>
+      <c r="L62" s="13">
+        <f t="shared" si="41"/>
+        <v>-1</v>
+      </c>
+      <c r="M62" s="13">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="N62" s="13"/>
+      <c r="O62" s="13">
+        <f t="shared" si="39"/>
+        <v>-1</v>
+      </c>
+      <c r="P62" s="13"/>
+      <c r="Q62" s="13"/>
+      <c r="S62">
+        <v>3.9512073636022903E-2</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="40"/>
+        <v>3.9512073636022903E-2</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="37"/>
+        <v>-3.9512073636022903E-2</v>
+      </c>
+      <c r="X62">
+        <f t="shared" si="37"/>
+        <v>3.9512073636022903E-2</v>
+      </c>
+      <c r="Y62">
+        <f t="shared" si="37"/>
+        <v>-3.9512073636022903E-2</v>
+      </c>
+      <c r="Z62">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA62">
+        <f t="shared" si="37"/>
+        <v>-3.9512073636022903E-2</v>
+      </c>
+      <c r="AB62">
+        <f t="shared" si="37"/>
+        <v>3.9512073636022903E-2</v>
+      </c>
+      <c r="AC62">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD62">
+        <f t="shared" si="37"/>
+        <v>-3.9512073636022903E-2</v>
+      </c>
+      <c r="AE62" s="13"/>
+      <c r="AF62" s="13"/>
+    </row>
+    <row r="63" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I63" s="13">
+        <v>1</v>
+      </c>
+      <c r="J63" s="13">
+        <v>-1</v>
+      </c>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13">
+        <f t="shared" si="41"/>
+        <v>-1</v>
+      </c>
+      <c r="M63" s="13">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="N63" s="13"/>
+      <c r="O63" s="13">
+        <f t="shared" si="39"/>
+        <v>-1</v>
+      </c>
+      <c r="P63" s="13"/>
+      <c r="Q63" s="13"/>
+      <c r="S63">
+        <v>0.21247080756198999</v>
+      </c>
+      <c r="V63">
+        <f t="shared" si="40"/>
+        <v>0.21247080756198999</v>
+      </c>
+      <c r="W63">
+        <f t="shared" si="37"/>
+        <v>-0.21247080756198999</v>
+      </c>
+      <c r="X63">
+        <f t="shared" si="37"/>
+        <v>0.21247080756198999</v>
+      </c>
+      <c r="Y63">
+        <f t="shared" si="37"/>
+        <v>-0.21247080756198999</v>
+      </c>
+      <c r="Z63">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA63">
+        <f t="shared" si="37"/>
+        <v>-0.21247080756198999</v>
+      </c>
+      <c r="AB63">
+        <f t="shared" si="37"/>
+        <v>0.21247080756198999</v>
+      </c>
+      <c r="AC63">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD63">
+        <f t="shared" si="37"/>
+        <v>-0.21247080756198999</v>
+      </c>
+      <c r="AE63" s="13"/>
+      <c r="AF63" s="13"/>
+    </row>
+    <row r="64" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64" s="13">
+        <v>1</v>
+      </c>
+      <c r="I64" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J64" s="13">
+        <v>1</v>
+      </c>
+      <c r="K64" s="13"/>
+      <c r="L64" s="13">
+        <f t="shared" si="41"/>
+        <v>-1</v>
+      </c>
+      <c r="M64" s="13">
+        <f>H64*J64</f>
+        <v>1</v>
+      </c>
+      <c r="N64" s="13"/>
+      <c r="O64" s="13">
+        <f t="shared" si="39"/>
+        <v>-1</v>
+      </c>
+      <c r="P64" s="13"/>
+      <c r="Q64" s="13"/>
+      <c r="S64" s="15">
+        <v>3.6208083767558102E-2</v>
+      </c>
+      <c r="V64">
+        <f t="shared" si="40"/>
+        <v>3.6208083767558102E-2</v>
+      </c>
+      <c r="W64">
+        <f t="shared" si="37"/>
+        <v>3.6208083767558102E-2</v>
+      </c>
+      <c r="X64">
+        <f t="shared" si="37"/>
+        <v>-3.6208083767558102E-2</v>
+      </c>
+      <c r="Y64">
+        <f t="shared" si="37"/>
+        <v>3.6208083767558102E-2</v>
+      </c>
+      <c r="Z64">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA64">
+        <f t="shared" si="37"/>
+        <v>-3.6208083767558102E-2</v>
+      </c>
+      <c r="AB64">
+        <f t="shared" si="37"/>
+        <v>3.6208083767558102E-2</v>
+      </c>
+      <c r="AC64">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD64">
+        <f t="shared" si="37"/>
+        <v>-3.6208083767558102E-2</v>
+      </c>
+      <c r="AE64" s="13"/>
+      <c r="AF64" s="13"/>
+    </row>
+    <row r="65" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B65" s="25"/>
       <c r="C65" s="25"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>17</v>
-      </c>
-      <c r="B66">
-        <v>4</v>
-      </c>
-      <c r="C66">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>1</v>
-      </c>
-      <c r="B67">
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65" s="13">
+        <v>1</v>
+      </c>
+      <c r="I65" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J65" s="13">
+        <v>1</v>
+      </c>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13">
+        <f t="shared" si="41"/>
+        <v>-1</v>
+      </c>
+      <c r="M65" s="13">
+        <f t="shared" ref="M65:M67" si="42">H65*J65</f>
+        <v>1</v>
+      </c>
+      <c r="N65" s="13"/>
+      <c r="O65" s="13">
+        <f t="shared" si="39"/>
+        <v>-1</v>
+      </c>
+      <c r="P65" s="13"/>
+      <c r="Q65" s="13"/>
+      <c r="S65">
+        <v>0.13742001360839101</v>
+      </c>
+      <c r="V65">
+        <f t="shared" si="40"/>
+        <v>0.13742001360839101</v>
+      </c>
+      <c r="W65">
+        <f t="shared" si="37"/>
+        <v>0.13742001360839101</v>
+      </c>
+      <c r="X65">
+        <f t="shared" si="37"/>
+        <v>-0.13742001360839101</v>
+      </c>
+      <c r="Y65">
+        <f t="shared" si="37"/>
+        <v>0.13742001360839101</v>
+      </c>
+      <c r="Z65">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA65">
+        <f t="shared" si="37"/>
+        <v>-0.13742001360839101</v>
+      </c>
+      <c r="AB65">
+        <f t="shared" si="37"/>
+        <v>0.13742001360839101</v>
+      </c>
+      <c r="AC65">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD65">
+        <f t="shared" si="37"/>
+        <v>-0.13742001360839101</v>
+      </c>
+      <c r="AE65" s="13"/>
+      <c r="AF65" s="13"/>
+    </row>
+    <row r="66" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66" s="13">
+        <v>1</v>
+      </c>
+      <c r="I66" s="13">
+        <v>1</v>
+      </c>
+      <c r="J66" s="13">
+        <v>-1</v>
+      </c>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="M66" s="13">
+        <f t="shared" si="42"/>
+        <v>-1</v>
+      </c>
+      <c r="N66" s="13"/>
+      <c r="O66" s="13">
+        <f t="shared" si="39"/>
+        <v>-1</v>
+      </c>
+      <c r="P66" s="13"/>
+      <c r="Q66" s="13"/>
+      <c r="S66">
+        <v>3.88719092150146E-2</v>
+      </c>
+      <c r="V66">
+        <f t="shared" si="40"/>
+        <v>3.88719092150146E-2</v>
+      </c>
+      <c r="W66">
+        <f t="shared" si="37"/>
+        <v>3.88719092150146E-2</v>
+      </c>
+      <c r="X66">
+        <f t="shared" si="37"/>
+        <v>3.88719092150146E-2</v>
+      </c>
+      <c r="Y66">
+        <f t="shared" si="37"/>
+        <v>-3.88719092150146E-2</v>
+      </c>
+      <c r="Z66">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA66">
+        <f t="shared" si="37"/>
+        <v>3.88719092150146E-2</v>
+      </c>
+      <c r="AB66">
+        <f t="shared" si="37"/>
+        <v>-3.88719092150146E-2</v>
+      </c>
+      <c r="AC66">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD66">
+        <f t="shared" si="37"/>
+        <v>-3.88719092150146E-2</v>
+      </c>
+      <c r="AE66" s="13"/>
+      <c r="AF66" s="13"/>
+    </row>
+    <row r="67" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67" s="13">
+        <v>1</v>
+      </c>
+      <c r="I67" s="13">
+        <v>1</v>
+      </c>
+      <c r="J67" s="13">
+        <v>1</v>
+      </c>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="M67" s="13">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+      <c r="N67" s="13"/>
+      <c r="O67" s="13">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13"/>
+      <c r="S67">
+        <v>0.211278284021195</v>
+      </c>
+      <c r="V67">
+        <f t="shared" si="40"/>
+        <v>0.211278284021195</v>
+      </c>
+      <c r="W67">
+        <f t="shared" si="37"/>
+        <v>0.211278284021195</v>
+      </c>
+      <c r="X67">
+        <f t="shared" si="37"/>
+        <v>0.211278284021195</v>
+      </c>
+      <c r="Y67">
+        <f t="shared" si="37"/>
+        <v>0.211278284021195</v>
+      </c>
+      <c r="Z67">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AA67">
+        <f t="shared" si="37"/>
+        <v>0.211278284021195</v>
+      </c>
+      <c r="AB67">
+        <f t="shared" si="37"/>
+        <v>0.211278284021195</v>
+      </c>
+      <c r="AC67">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AD67">
+        <f t="shared" si="37"/>
+        <v>0.211278284021195</v>
+      </c>
+      <c r="AE67" s="13"/>
+      <c r="AF67" s="13"/>
+    </row>
+    <row r="68" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="69" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F69" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G69" s="20">
+        <f>SUM(S52:S67)</f>
+        <v>2.31304422075792</v>
+      </c>
+      <c r="H69" s="20">
+        <f>SUM(W52:W67)</f>
+        <v>3.2738746266204405E-2</v>
+      </c>
+      <c r="I69" s="20">
+        <f t="shared" ref="I69:O69" si="43">SUM(X52:X67)</f>
+        <v>0.76190136134787556</v>
+      </c>
+      <c r="J69" s="20">
+        <f t="shared" si="43"/>
+        <v>1.1543255625859719</v>
+      </c>
+      <c r="K69" s="20">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L69" s="20">
+        <f t="shared" si="43"/>
+        <v>2.0621053205794521E-2</v>
+      </c>
+      <c r="M69" s="20">
+        <f t="shared" si="43"/>
+        <v>0.53549716676591197</v>
+      </c>
+      <c r="N69" s="20">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="O69" s="20">
+        <f t="shared" si="43"/>
+        <v>0.36173134179273203</v>
+      </c>
+      <c r="P69" s="20"/>
+      <c r="Q69" s="20"/>
+      <c r="R69" s="22"/>
+    </row>
+    <row r="70" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="F70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G70">
+        <f>G69/16</f>
+        <v>0.14456526379737</v>
+      </c>
+      <c r="H70">
+        <f>H69/16</f>
+        <v>2.0461716416377753E-3</v>
+      </c>
+      <c r="I70">
+        <f t="shared" ref="I70:O70" si="44">I69/16</f>
+        <v>4.7618835084242223E-2</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="44"/>
+        <v>7.2145347661623241E-2</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="44"/>
+        <v>1.2888158253621575E-3</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="44"/>
+        <v>3.3468572922869498E-2</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="44"/>
+        <v>2.2608208862045752E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
         <v>15</v>
       </c>
-      <c r="C67">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>2</v>
-      </c>
-      <c r="B68">
-        <v>25</v>
-      </c>
-      <c r="C68">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D74" t="s">
-        <v>12</v>
-      </c>
-      <c r="E74" t="s">
-        <v>13</v>
-      </c>
-      <c r="F74" t="s">
-        <v>14</v>
-      </c>
-      <c r="G74" t="s">
-        <v>15</v>
-      </c>
-      <c r="H74" t="s">
-        <v>16</v>
-      </c>
-      <c r="I74" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D75">
-        <f>K2</f>
-        <v>-1</v>
-      </c>
-      <c r="E75">
-        <f>H2*B67</f>
-        <v>-15</v>
-      </c>
-      <c r="F75">
-        <f>B67*I2</f>
-        <v>-15</v>
-      </c>
-      <c r="G75">
-        <f>K2*J2</f>
-        <v>1</v>
-      </c>
-      <c r="H75">
-        <v>15</v>
-      </c>
-      <c r="I75" t="e">
-        <f>(H75-#REF!)^2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
-        <v>19</v>
-      </c>
-      <c r="C76">
-        <f>AVERAGE(H75:H78)</f>
-        <v>40</v>
-      </c>
-      <c r="D76">
-        <f>K3</f>
-        <v>-1</v>
-      </c>
-      <c r="E76">
-        <f>H3*C67</f>
-        <v>-45</v>
-      </c>
-      <c r="F76">
-        <f xml:space="preserve"> C67*I3</f>
-        <v>-45</v>
-      </c>
-      <c r="G76">
-        <f>K3*J3</f>
-        <v>-1</v>
-      </c>
-      <c r="H76">
-        <v>45</v>
-      </c>
-      <c r="I76" t="e">
-        <f>(H76-#REF!)^2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D77">
-        <f>K4</f>
-        <v>-1</v>
-      </c>
-      <c r="E77">
-        <f>H4*B68</f>
-        <v>-25</v>
-      </c>
-      <c r="F77">
-        <f>B68*I4</f>
-        <v>25</v>
-      </c>
-      <c r="G77">
-        <f>K4*J4</f>
-        <v>1</v>
-      </c>
-      <c r="H77">
-        <v>25</v>
-      </c>
-      <c r="I77" t="e">
-        <f>(H77-#REF!)^2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D78">
-        <f>K5</f>
-        <v>-1</v>
-      </c>
-      <c r="E78">
-        <f>C68*H5</f>
-        <v>-75</v>
-      </c>
-      <c r="F78">
-        <f>C68*I5</f>
-        <v>75</v>
-      </c>
-      <c r="G78">
-        <f>K5*J5</f>
-        <v>-1</v>
-      </c>
-      <c r="H78">
-        <v>75</v>
-      </c>
-      <c r="I78" t="e">
-        <f>(H78-#REF!)^2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D79" s="2">
-        <f>SUM(D75:D78)</f>
-        <v>-4</v>
-      </c>
-      <c r="E79" s="3">
-        <f>SUM(E75:E78)</f>
-        <v>-160</v>
-      </c>
-      <c r="F79" s="3">
-        <f>SUM(F75:F78)</f>
-        <v>40</v>
-      </c>
-      <c r="G79" s="4">
-        <f>SUM(G75:G78)</f>
+      <c r="H71">
+        <f>4*(H70)^2</f>
+        <v>1.6747273548170512E-5</v>
+      </c>
+      <c r="I71">
+        <f t="shared" ref="I71:Q71" si="45">4*(I70)^2</f>
+        <v>9.070213819121032E-3</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="45"/>
+        <v>2.0819804756865946E-2</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="45"/>
+        <v>6.6441849268157575E-6</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="45"/>
+        <v>4.4805814939737334E-3</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="45"/>
+        <v>2.0445244317995365E-3</v>
+      </c>
+      <c r="R71" t="s">
+        <v>59</v>
+      </c>
+      <c r="S71">
+        <f>SUM(H71:O71)</f>
+        <v>3.6438515960235236E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="F72" t="s">
+        <v>56</v>
+      </c>
+      <c r="H72">
+        <f>(H71/$S$71)*100</f>
+        <v>4.5960361191565928E-2</v>
+      </c>
+      <c r="I72">
+        <f t="shared" ref="I72:O72" si="46">(I71/$S$71)*100</f>
+        <v>24.891831020284169</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="46"/>
+        <v>57.136807601018283</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="H79" t="s">
-        <v>20</v>
-      </c>
-      <c r="I79" t="e">
-        <f>SUM(I75:I78)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D80">
-        <f>D79/4</f>
-        <v>-1</v>
-      </c>
-      <c r="E80">
-        <f>E79/4</f>
-        <v>-40</v>
-      </c>
-      <c r="F80">
-        <f>F79/4</f>
-        <v>10</v>
-      </c>
-      <c r="G80">
-        <f>G79/4</f>
+      <c r="L72">
+        <f t="shared" si="46"/>
+        <v>1.823396137775328E-2</v>
+      </c>
+      <c r="M72">
+        <f t="shared" si="46"/>
+        <v>12.296278747639777</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D82" t="s">
-        <v>21</v>
-      </c>
-      <c r="F82">
-        <f>4*E80^2</f>
-        <v>6400</v>
-      </c>
-      <c r="G82">
-        <f>4*F80^2</f>
-        <v>400</v>
-      </c>
-      <c r="H82">
-        <f>4*G80^2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F83" t="e">
-        <f>F82/#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G83" t="e">
-        <f>G82/#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H83" t="e">
-        <f>H82/#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E84" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F84" s="6" t="e">
-        <f>F83*100</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G84" s="6" t="e">
-        <f>G83*100</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H84" s="7" t="e">
-        <f>H83*100</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>23</v>
-      </c>
-      <c r="L96" s="24" t="s">
-        <v>24</v>
-      </c>
+      <c r="O72">
+        <f t="shared" si="46"/>
+        <v>5.6108883084884491</v>
+      </c>
+    </row>
+    <row r="78" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="79" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D79" s="2"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="4"/>
+    </row>
+    <row r="83" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="84" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E84" s="5"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="7"/>
+    </row>
+    <row r="96" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="L96" s="24"/>
       <c r="M96" s="24"/>
       <c r="N96" s="24"/>
     </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B97" t="s">
-        <v>12</v>
-      </c>
-      <c r="C97" t="s">
-        <v>13</v>
-      </c>
-      <c r="D97" t="s">
-        <v>14</v>
-      </c>
-      <c r="E97" t="s">
-        <v>15</v>
-      </c>
-      <c r="F97" t="s">
-        <v>25</v>
-      </c>
-      <c r="G97" t="s">
-        <v>26</v>
-      </c>
-      <c r="H97" t="s">
-        <v>27</v>
-      </c>
-      <c r="I97" t="s">
-        <v>28</v>
-      </c>
-      <c r="L97" t="s">
-        <v>29</v>
-      </c>
-      <c r="M97" t="s">
-        <v>30</v>
-      </c>
-      <c r="N97" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B98">
-        <v>1</v>
-      </c>
-      <c r="C98">
-        <v>-1</v>
-      </c>
-      <c r="D98">
-        <v>-1</v>
-      </c>
-      <c r="E98">
-        <v>1</v>
-      </c>
-      <c r="F98">
-        <v>15</v>
-      </c>
-      <c r="G98">
-        <v>18</v>
-      </c>
-      <c r="H98">
-        <v>12</v>
-      </c>
-      <c r="I98">
-        <f>AVERAGE(F98:H98)</f>
-        <v>15</v>
-      </c>
-      <c r="L98">
-        <f t="shared" ref="L98:N101" si="37">F98-$I98</f>
-        <v>0</v>
-      </c>
-      <c r="M98">
-        <f t="shared" si="37"/>
-        <v>3</v>
-      </c>
-      <c r="N98">
-        <f t="shared" si="37"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B99">
-        <v>1</v>
-      </c>
-      <c r="C99">
-        <v>1</v>
-      </c>
-      <c r="D99">
-        <v>-1</v>
-      </c>
-      <c r="E99">
-        <v>-1</v>
-      </c>
-      <c r="F99">
-        <v>45</v>
-      </c>
-      <c r="G99">
-        <v>48</v>
-      </c>
-      <c r="H99">
-        <v>51</v>
-      </c>
-      <c r="I99">
-        <f t="shared" ref="I99:I101" si="38">AVERAGE(F99:H99)</f>
-        <v>48</v>
-      </c>
-      <c r="L99">
-        <f t="shared" si="37"/>
-        <v>-3</v>
-      </c>
-      <c r="M99">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-      <c r="N99">
-        <f t="shared" si="37"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B100">
-        <v>1</v>
-      </c>
-      <c r="C100">
-        <v>-1</v>
-      </c>
-      <c r="D100">
-        <v>1</v>
-      </c>
-      <c r="E100">
-        <v>-1</v>
-      </c>
-      <c r="F100">
-        <v>25</v>
-      </c>
-      <c r="G100">
-        <v>28</v>
-      </c>
-      <c r="H100">
-        <v>19</v>
-      </c>
-      <c r="I100">
-        <f t="shared" si="38"/>
-        <v>24</v>
-      </c>
-      <c r="L100">
-        <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="M100">
-        <f t="shared" si="37"/>
-        <v>4</v>
-      </c>
-      <c r="N100">
-        <f t="shared" si="37"/>
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B101">
-        <v>1</v>
-      </c>
-      <c r="C101">
-        <v>1</v>
-      </c>
-      <c r="D101">
-        <v>1</v>
-      </c>
-      <c r="E101">
-        <v>1</v>
-      </c>
-      <c r="F101">
-        <v>75</v>
-      </c>
-      <c r="G101">
-        <v>75</v>
-      </c>
-      <c r="H101">
-        <v>81</v>
-      </c>
-      <c r="I101">
-        <f t="shared" si="38"/>
-        <v>77</v>
-      </c>
-      <c r="L101">
-        <f t="shared" si="37"/>
-        <v>-2</v>
-      </c>
-      <c r="M101">
-        <f t="shared" si="37"/>
-        <v>-2</v>
-      </c>
-      <c r="N101">
-        <f t="shared" si="37"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="L102">
-        <f>SUM(L98:L101)</f>
-        <v>-4</v>
-      </c>
-      <c r="M102">
-        <f t="shared" ref="M102:N102" si="39">SUM(M98:M101)</f>
-        <v>5</v>
-      </c>
-      <c r="N102">
-        <f t="shared" si="39"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="L103">
-        <f>L102/4</f>
-        <v>-1</v>
-      </c>
-      <c r="M103">
-        <f t="shared" ref="M103:N103" si="40">M102/4</f>
-        <v>1.25</v>
-      </c>
-      <c r="N103">
-        <f t="shared" si="40"/>
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N104" s="8">
-        <f>SUM(L98^2+M98^2+N98^2+L99^2+M99^2+N99^2+L100^2+M100^2+N100^2+L101^2+M101^2+N101^2)</f>
-        <v>102</v>
-      </c>
-    </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="F105" t="s">
-        <v>12</v>
-      </c>
-      <c r="G105" t="s">
-        <v>13</v>
-      </c>
-      <c r="H105" t="s">
-        <v>14</v>
-      </c>
-      <c r="I105" t="s">
-        <v>15</v>
-      </c>
-      <c r="J105" t="s">
-        <v>28</v>
-      </c>
-      <c r="N105">
-        <f>N104/K110</f>
-        <v>1.4505119453924915E-2</v>
-      </c>
-    </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="F106">
-        <f>J106*B98</f>
-        <v>15</v>
-      </c>
-      <c r="G106">
-        <f t="shared" ref="G106:I109" si="41">C98*$J106</f>
-        <v>-15</v>
-      </c>
-      <c r="H106">
-        <f t="shared" si="41"/>
-        <v>-15</v>
-      </c>
-      <c r="I106">
-        <f t="shared" si="41"/>
-        <v>15</v>
-      </c>
-      <c r="J106">
-        <v>15</v>
-      </c>
-      <c r="N106">
-        <f>N105*100</f>
-        <v>1.4505119453924915</v>
-      </c>
-    </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C107" t="s">
-        <v>19</v>
-      </c>
-      <c r="D107">
-        <f>AVERAGE(J106:J109)</f>
-        <v>41</v>
-      </c>
-      <c r="F107">
-        <f t="shared" ref="F107:F109" si="42">J107*B99</f>
-        <v>48</v>
-      </c>
-      <c r="G107">
-        <f t="shared" si="41"/>
-        <v>48</v>
-      </c>
-      <c r="H107">
-        <f t="shared" si="41"/>
-        <v>-48</v>
-      </c>
-      <c r="I107">
-        <f t="shared" si="41"/>
-        <v>-48</v>
-      </c>
-      <c r="J107">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="F108">
-        <f t="shared" si="42"/>
-        <v>24</v>
-      </c>
-      <c r="G108">
-        <f t="shared" si="41"/>
-        <v>-24</v>
-      </c>
-      <c r="H108">
-        <f t="shared" si="41"/>
-        <v>24</v>
-      </c>
-      <c r="I108">
-        <f t="shared" si="41"/>
-        <v>-24</v>
-      </c>
-      <c r="J108">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="109" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F109">
-        <f t="shared" si="42"/>
-        <v>77</v>
-      </c>
-      <c r="G109">
-        <f t="shared" si="41"/>
-        <v>77</v>
-      </c>
-      <c r="H109">
-        <f t="shared" si="41"/>
-        <v>77</v>
-      </c>
-      <c r="I109">
-        <f t="shared" si="41"/>
-        <v>77</v>
-      </c>
-      <c r="J109">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="110" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F110" s="2">
-        <f>SUM(F106:F109)</f>
-        <v>164</v>
-      </c>
-      <c r="G110" s="3">
-        <f>SUM(G106:G109)</f>
-        <v>86</v>
-      </c>
-      <c r="H110" s="3">
-        <f>SUM(H106:H109)</f>
-        <v>38</v>
-      </c>
-      <c r="I110" s="4">
-        <f>SUM(I106:I109)</f>
-        <v>20</v>
-      </c>
-      <c r="J110" t="s">
-        <v>32</v>
-      </c>
-      <c r="K110">
-        <f>SUM(N104,G113:I113)</f>
-        <v>7032</v>
-      </c>
-    </row>
-    <row r="111" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="F111">
-        <f>F110/4</f>
-        <v>41</v>
-      </c>
-      <c r="G111">
-        <f t="shared" ref="G111:I111" si="43">G110/4</f>
-        <v>21.5</v>
-      </c>
-      <c r="H111">
-        <f t="shared" si="43"/>
-        <v>9.5</v>
-      </c>
-      <c r="I111">
-        <f t="shared" si="43"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E113" t="s">
-        <v>33</v>
-      </c>
-      <c r="G113">
-        <f>4*3*G111^2</f>
-        <v>5547</v>
-      </c>
-      <c r="H113">
-        <f t="shared" ref="H113:I113" si="44">4*3*H111^2</f>
-        <v>1083</v>
-      </c>
-      <c r="I113">
-        <f t="shared" si="44"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G114" t="e">
-        <f>G113/$K$103</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H114" t="e">
-        <f>H113/$K$103</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I114" t="e">
-        <f>I113/$K$103</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
+    <row r="104" spans="6:14" x14ac:dyDescent="0.3">
+      <c r="N104" s="8"/>
+    </row>
+    <row r="109" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="110" spans="6:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F110" s="2"/>
+      <c r="G110" s="3"/>
+      <c r="H110" s="3"/>
+      <c r="I110" s="4"/>
+    </row>
+    <row r="114" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="115" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F115" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G115" s="9" t="e">
-        <f>G114*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H115" s="9" t="e">
-        <f t="shared" ref="H115:I115" si="45">H114*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I115" s="9" t="e">
-        <f t="shared" si="45"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F115" s="5"/>
+      <c r="G115" s="9"/>
+      <c r="H115" s="9"/>
+      <c r="I115" s="9"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
@@ -6583,181 +7300,181 @@
         <v>-3</v>
       </c>
       <c r="C119">
-        <f t="shared" ref="C119:C129" si="46">_xlfn.NORM.S.INV(D119)</f>
+        <f t="shared" ref="C119:C129" si="47">_xlfn.NORM.S.INV(D119)</f>
         <v>-1.1503493803760083</v>
       </c>
       <c r="D119" s="10">
-        <f t="shared" ref="D119:D129" si="47">(A119-0.5)/12</f>
+        <f t="shared" ref="D119:D129" si="48">(A119-0.5)/12</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120">
-        <f t="shared" ref="A120:A129" si="48">A119+1</f>
+        <f t="shared" ref="A120:A129" si="49">A119+1</f>
         <v>3</v>
       </c>
       <c r="B120">
         <v>-3</v>
       </c>
       <c r="C120">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-0.81221780149991241</v>
       </c>
       <c r="D120" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>4</v>
       </c>
       <c r="B121">
         <v>-2</v>
       </c>
       <c r="C121">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-0.54852228269809788</v>
       </c>
       <c r="D121" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>5</v>
       </c>
       <c r="B122">
         <v>-2</v>
       </c>
       <c r="C122">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-0.3186393639643752</v>
       </c>
       <c r="D122" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.375</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>6</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="C123">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>-0.10463345561407539</v>
       </c>
       <c r="D123" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>7</v>
       </c>
       <c r="B124">
         <v>0</v>
       </c>
       <c r="C124">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.10463345561407525</v>
       </c>
       <c r="D124" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125">
+        <f t="shared" si="49"/>
+        <v>8</v>
+      </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="47"/>
+        <v>0.3186393639643752</v>
+      </c>
+      <c r="D125" s="10">
         <f t="shared" si="48"/>
-        <v>8</v>
-      </c>
-      <c r="B125">
-        <v>1</v>
-      </c>
-      <c r="C125">
-        <f t="shared" si="46"/>
-        <v>0.3186393639643752</v>
-      </c>
-      <c r="D125" s="10">
-        <f t="shared" si="47"/>
         <v>0.625</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>9</v>
       </c>
       <c r="B126">
         <v>3</v>
       </c>
       <c r="C126">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.54852228269809822</v>
       </c>
       <c r="D126" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>10</v>
       </c>
       <c r="B127">
         <v>3</v>
       </c>
       <c r="C127">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.81221780149991241</v>
       </c>
       <c r="D127" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>11</v>
       </c>
       <c r="B128">
         <v>4</v>
       </c>
       <c r="C128">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>1.1503493803760083</v>
       </c>
       <c r="D128" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.875</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>12</v>
       </c>
       <c r="B129">
         <v>4</v>
       </c>
       <c r="C129">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>1.7316643961222455</v>
       </c>
       <c r="D129" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0.95833333333333337</v>
       </c>
     </row>
@@ -6892,7 +7609,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -6930,7 +7647,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -6944,7 +7661,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -6952,18 +7669,18 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B8" s="24"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -6971,97 +7688,97 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>400</v>
       </c>
-      <c r="J11" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
+      <c r="J11" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
-      <c r="J12" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q12" s="27"/>
+      <c r="J12" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="31"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="G13" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
+      <c r="G13" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
       <c r="J13" s="16" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="Q13" s="16" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
+      <c r="D14" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
       <c r="J14" s="15">
         <v>7.5307516287585405E-2</v>
       </c>
@@ -7088,11 +7805,11 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D15" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
+      <c r="D15" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -7122,9 +7839,9 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -7138,9 +7855,9 @@
       <c r="Q16" s="17"/>
     </row>
     <row r="17" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -7155,18 +7872,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:Q12"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="D15:F15"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>